<commit_message>
Applied fixes: FHIR-37352. Updated the source example data spreadsheet with a correction to typo in ICD10 code.
</commit_message>
<xml_diff>
--- a/input/images/Source/Risk Adjustment IG Test Data 2022 01 11.xlsx
+++ b/input/images/Source/Risk Adjustment IG Test Data 2022 01 11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmicha2\Downloads\davinci-ra\input\images\Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\davinci-ra\input\images\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26736DA5-09C7-4220-854F-27EC3BA3B9BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3650B7-9AF1-422E-9B04-A4F45DB5DADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A7B2BBE4-BD46-48EE-98EF-4DA09EA82077}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" activeTab="1" xr2:uid="{A7B2BBE4-BD46-48EE-98EF-4DA09EA82077}"/>
   </bookViews>
   <sheets>
     <sheet name="Gaps" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="195">
   <si>
     <t>Family Name</t>
   </si>
@@ -671,6 +671,12 @@
   </si>
   <si>
     <t>obs2</t>
+  </si>
+  <si>
+    <t>E1151</t>
+  </si>
+  <si>
+    <t>5/20/2022 Note: corrected typo from I1151 to E11.51</t>
   </si>
 </sst>
 </file>
@@ -854,7 +860,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -969,6 +975,22 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3595,7 +3617,7 @@
   <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5221,50 +5243,50 @@
       <c r="P36" s="31"/>
       <c r="Q36" s="31"/>
     </row>
-    <row r="37" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="25">
+    <row r="37" spans="1:17" s="49" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="45">
         <v>39</v>
       </c>
-      <c r="B37" s="26">
+      <c r="B37" s="46">
         <v>44239</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="E37" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="F37" s="27" t="s">
+      <c r="F37" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="G37" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="H37" s="27">
+      <c r="G37" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="H37" s="47">
         <v>216</v>
       </c>
-      <c r="I37" s="27" t="s">
+      <c r="I37" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="31" t="s">
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="M37" s="31">
+      <c r="M37" s="48">
         <v>6</v>
       </c>
-      <c r="N37" s="43">
+      <c r="N37" s="48">
         <v>35</v>
       </c>
-      <c r="O37" s="31">
+      <c r="O37" s="48">
         <v>35</v>
       </c>
-      <c r="P37" s="31"/>
-      <c r="Q37" s="31"/>
+      <c r="P37" s="48"/>
+      <c r="Q37" s="48"/>
     </row>
     <row r="38" spans="1:17" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="25">
@@ -5526,6 +5548,9 @@
       <c r="F47">
         <v>1</v>
       </c>
+      <c r="G47" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" t="s">

</xml_diff>